<commit_message>
Bonn Bug Fixes + 2 New Code Lists
- Added Amt "0", Produktbereich "0"
- Added raw data for 3 code lists
- Updated DSD
</commit_message>
<xml_diff>
--- a/Bonn/raw/Aemterhierarchie.xlsx
+++ b/Bonn/raw/Aemterhierarchie.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ok-server\EIS-Homes\cengels\Eigene Dateien\OpenBudgets.eu\DataSets\SampleData\Bonn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ok-server\eis-homes\cengels\Desktop\GitHub\OpenBudgets\datasets\Bonn\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t>Amt</t>
   </si>
@@ -53,25 +53,7 @@
     <t>Amt 11</t>
   </si>
   <si>
-    <t>Amt 20, Abteilung 1</t>
-  </si>
-  <si>
-    <t>Amt 20, Abteilung 2</t>
-  </si>
-  <si>
-    <t>Amt 21, Abteilung 2</t>
-  </si>
-  <si>
     <t>Amt 23</t>
-  </si>
-  <si>
-    <t>Amt 25</t>
-  </si>
-  <si>
-    <t>Amt 41, Abteilung 9</t>
-  </si>
-  <si>
-    <t>Amt 70</t>
   </si>
   <si>
     <t>Ziffer23</t>
@@ -278,6 +260,33 @@
   </si>
   <si>
     <t>Koordination Integration, Arbeitssicherheit, Beethoven 2020, Konferenzzentrum/Beethovenhalle</t>
+  </si>
+  <si>
+    <t>veraltet</t>
+  </si>
+  <si>
+    <t>Haushaltsmanagement</t>
+  </si>
+  <si>
+    <t>Beteiligungsverwaltung</t>
+  </si>
+  <si>
+    <t>Steueramt</t>
+  </si>
+  <si>
+    <t>Referat Vergabedienste</t>
+  </si>
+  <si>
+    <t>Zentrale Vergabedienstleistungen</t>
+  </si>
+  <si>
+    <t>Theater</t>
+  </si>
+  <si>
+    <t>Koordinierungsstelle</t>
+  </si>
+  <si>
+    <t>Ämterübergreifend</t>
   </si>
 </sst>
 </file>
@@ -359,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -375,6 +384,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -657,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,10 +688,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -687,201 +700,192 @@
         <v>1</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7">
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
         <v>100</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>200</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>200</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
         <v>300</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
         <v>400</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1000</v>
-      </c>
       <c r="D6" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>10</v>
       </c>
       <c r="B7" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C7" s="7">
-        <v>1020</v>
+        <v>1000</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1000</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>10</v>
       </c>
       <c r="B8" s="6">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7">
-        <v>1066</v>
+        <v>1020</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="4">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>10</v>
       </c>
       <c r="B9" s="6">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C9" s="7">
-        <v>1077</v>
+        <v>1066</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="4">
         <v>1000</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>10</v>
       </c>
       <c r="B10" s="6">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C10" s="7">
-        <v>1088</v>
+        <v>1077</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" s="4">
         <v>1000</v>
       </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="6">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C11" s="7">
-        <v>1099</v>
+        <v>1088</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="4">
         <v>1000</v>
@@ -889,71 +893,75 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="C12" s="7">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1000</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="6">
         <v>0</v>
       </c>
       <c r="C13" s="7">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="6">
         <v>0</v>
       </c>
       <c r="C14" s="7">
-        <v>1400</v>
+        <v>1300</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6">
         <v>0</v>
       </c>
       <c r="C15" s="7">
-        <v>2000</v>
+        <v>1400</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F15" s="4"/>
     </row>
@@ -962,278 +970,286 @@
         <v>20</v>
       </c>
       <c r="B16" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C16" s="7">
-        <v>2010</v>
+        <v>2000</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="4">
-        <v>2000</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>20</v>
       </c>
       <c r="B17" s="6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C17" s="7">
-        <v>2020</v>
+        <v>2010</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="8"/>
+        <v>79</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="F17" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C18" s="7">
-        <v>2100</v>
+        <v>2020</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>21</v>
       </c>
       <c r="B19" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C19" s="7">
-        <v>2120</v>
+        <v>2100</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="4">
-        <v>2100</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C20" s="7">
-        <v>2300</v>
+        <v>2120</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="4">
+        <v>2100</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
+        <v>23</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2300</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
         <v>25</v>
       </c>
-      <c r="B21" s="6">
-        <v>0</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="B22" s="6">
+        <v>0</v>
+      </c>
+      <c r="C22" s="7">
         <v>2500</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="D22" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>30</v>
       </c>
-      <c r="B22" s="6">
-        <v>0</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="B23" s="6">
+        <v>0</v>
+      </c>
+      <c r="C23" s="7">
         <v>3000</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>33</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7">
+        <v>3300</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
         <v>37</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+      <c r="C25" s="7">
+        <v>3700</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>40</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7">
+        <v>4000</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>33</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="7">
-        <v>3300</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>37</v>
-      </c>
-      <c r="B24" s="6">
-        <v>0</v>
-      </c>
-      <c r="C24" s="7">
-        <v>3700</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>40</v>
-      </c>
-      <c r="B25" s="6">
-        <v>0</v>
-      </c>
-      <c r="C25" s="7">
-        <v>4000</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>41</v>
-      </c>
-      <c r="B26" s="6">
-        <v>0</v>
-      </c>
-      <c r="C26" s="7">
-        <v>4100</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>41</v>
       </c>
       <c r="B27" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C27" s="7">
-        <v>4120</v>
+        <v>4100</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" s="4">
-        <v>4100</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>41</v>
       </c>
       <c r="B28" s="6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C28" s="7">
-        <v>4130</v>
+        <v>4120</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F28" s="4">
         <v>4100</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>41</v>
       </c>
       <c r="B29" s="6">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C29" s="7">
-        <v>4140</v>
+        <v>4130</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F29" s="4">
         <v>4100</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>41</v>
       </c>
       <c r="B30" s="6">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C30" s="7">
-        <v>4150</v>
+        <v>4140</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F30" s="4">
         <v>4100</v>
@@ -1244,16 +1260,16 @@
         <v>41</v>
       </c>
       <c r="B31" s="6">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C31" s="7">
-        <v>4160</v>
+        <v>4150</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F31" s="4">
         <v>4100</v>
@@ -1264,16 +1280,16 @@
         <v>41</v>
       </c>
       <c r="B32" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C32" s="7">
-        <v>4170</v>
+        <v>4160</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F32" s="4">
         <v>4100</v>
@@ -1284,16 +1300,16 @@
         <v>41</v>
       </c>
       <c r="B33" s="6">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C33" s="7">
-        <v>4180</v>
+        <v>4170</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F33" s="4">
         <v>4100</v>
@@ -1304,256 +1320,262 @@
         <v>41</v>
       </c>
       <c r="B34" s="6">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C34" s="7">
-        <v>4190</v>
+        <v>4180</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="8"/>
+        <v>50</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="F34" s="4">
         <v>4100</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="3" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
+        <v>41</v>
+      </c>
+      <c r="B35" s="6">
+        <v>90</v>
+      </c>
+      <c r="C35" s="7">
+        <v>4190</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="4">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="3" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
         <v>50</v>
       </c>
-      <c r="B35" s="6">
-        <v>0</v>
-      </c>
-      <c r="C35" s="7">
+      <c r="B36" s="6">
+        <v>0</v>
+      </c>
+      <c r="C36" s="7">
         <v>5000</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
+      <c r="D36" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
         <v>51</v>
       </c>
-      <c r="B36" s="6">
-        <v>0</v>
-      </c>
-      <c r="C36" s="7">
+      <c r="B37" s="6">
+        <v>0</v>
+      </c>
+      <c r="C37" s="7">
         <v>5100</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
-        <v>52</v>
-      </c>
-      <c r="B37" s="6">
-        <v>0</v>
-      </c>
-      <c r="C37" s="7">
-        <v>5200</v>
-      </c>
       <c r="D37" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="6">
         <v>0</v>
       </c>
       <c r="C38" s="7">
-        <v>5300</v>
+        <v>5200</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
+        <v>53</v>
+      </c>
+      <c r="B39" s="6">
+        <v>0</v>
+      </c>
+      <c r="C39" s="7">
+        <v>5300</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="6">
-        <v>0</v>
-      </c>
-      <c r="C39" s="7">
-        <v>5600</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="E39" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B40" s="6">
         <v>0</v>
       </c>
       <c r="C40" s="7">
-        <v>6100</v>
+        <v>5600</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
+        <v>61</v>
+      </c>
+      <c r="B41" s="6">
+        <v>0</v>
+      </c>
+      <c r="C41" s="7">
+        <v>6100</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
         <v>62</v>
       </c>
-      <c r="B41" s="6">
-        <v>0</v>
-      </c>
-      <c r="C41" s="7">
+      <c r="B42" s="6">
+        <v>0</v>
+      </c>
+      <c r="C42" s="7">
         <v>6200</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D42" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>63</v>
+      </c>
+      <c r="B43" s="6">
+        <v>0</v>
+      </c>
+      <c r="C43" s="7">
+        <v>6300</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E41" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>66</v>
+      </c>
+      <c r="B44" s="6">
+        <v>0</v>
+      </c>
+      <c r="C44" s="7">
+        <v>6600</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>68</v>
+      </c>
+      <c r="B45" s="6">
+        <v>0</v>
+      </c>
+      <c r="C45" s="7">
+        <v>6800</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="6">
-        <v>0</v>
-      </c>
-      <c r="C42" s="7">
-        <v>6300</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F42" s="4"/>
-    </row>
-    <row r="43" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
-        <v>66</v>
-      </c>
-      <c r="B43" s="6">
-        <v>0</v>
-      </c>
-      <c r="C43" s="7">
-        <v>6600</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="8" t="s">
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
         <v>70</v>
       </c>
-      <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
-        <v>68</v>
-      </c>
-      <c r="B44" s="6">
-        <v>0</v>
-      </c>
-      <c r="C44" s="7">
-        <v>6800</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F44" s="4"/>
-    </row>
-    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
-        <v>70</v>
-      </c>
-      <c r="B45" s="6">
-        <v>0</v>
-      </c>
-      <c r="C45" s="7">
+      <c r="B46" s="6">
+        <v>0</v>
+      </c>
+      <c r="C46" s="7">
         <v>7000</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
-        <v>90</v>
-      </c>
-      <c r="B46" s="6">
-        <v>0</v>
-      </c>
-      <c r="C46" s="7">
-        <v>9000</v>
-      </c>
       <c r="D46" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>90</v>
       </c>
       <c r="B47" s="6">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C47" s="7">
-        <v>9040</v>
+        <v>9000</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F47" s="4"/>
     </row>
@@ -1562,18 +1584,36 @@
         <v>90</v>
       </c>
       <c r="B48" s="6">
+        <v>40</v>
+      </c>
+      <c r="C48" s="7">
+        <v>9040</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>90</v>
+      </c>
+      <c r="B49" s="6">
         <v>60</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C49" s="7">
         <v>9060</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F48" s="4"/>
+      <c r="D49" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F49" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A3:L241">

</xml_diff>